<commit_message>
Work on param parser and rest of SKUs upload
</commit_message>
<xml_diff>
--- a/test/fixtures/files/ISTC_March_2017_basic_text.xlsx
+++ b/test/fixtures/files/ISTC_March_2017_basic_text.xlsx
@@ -66,11 +66,12 @@
     <t>Broders Cucina Italiana</t>
   </si>
   <si>
-    <t>PAS12003</t>
+    <t>OLI00134</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>OLI1000</t>
+    <t>PAS12000</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -491,11 +492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="11"/>
@@ -579,7 +580,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
@@ -607,7 +608,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6">
         <v>20</v>
@@ -635,7 +636,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="6">
         <v>20</v>
@@ -693,12 +694,9 @@
         <v>61.012658227848107</v>
       </c>
     </row>
-    <row r="32" ht="15"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="1.25" bottom="0.65277777777777779" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;"Arial"&amp;12&amp;BGustiamo, Inc.&amp;B
 &amp;11&amp;BItems Sold to Customers&amp;B

</xml_diff>